<commit_message>
Update AE1 Marking Sheet - In use.xlsx
</commit_message>
<xml_diff>
--- a/AE1 Marking Sheet - In use.xlsx
+++ b/AE1 Marking Sheet - In use.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18107AD-2313-4BB2-A000-F0DBFEB4F849}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4317E5B1-C59A-4388-812F-BD902844B89C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -535,16 +535,16 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2124,8 +2124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64:D64"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,19 +2136,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="10"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="6">
         <v>3</v>
       </c>
@@ -2157,136 +2157,136 @@
       <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>1</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>2</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>3</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="6"/>
     </row>
     <row r="11" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>1</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>2</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>3</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="8"/>
+      <c r="C14" s="7"/>
       <c r="D14" s="6"/>
     </row>
     <row r="15" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>1</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>2</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>3</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="8"/>
+      <c r="C18" s="7"/>
       <c r="D18" s="6">
         <v>2</v>
       </c>
@@ -2295,34 +2295,34 @@
       <c r="B19" s="2">
         <v>1</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>2</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>3</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="7"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="8"/>
+      <c r="C22" s="7"/>
       <c r="D22" s="6">
         <v>3</v>
       </c>
@@ -2331,96 +2331,96 @@
       <c r="B23" s="2">
         <v>1</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="7"/>
+      <c r="D23" s="9"/>
     </row>
     <row r="24" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>2</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="7"/>
+      <c r="D24" s="9"/>
     </row>
     <row r="25" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>3</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="8"/>
+      <c r="C26" s="7"/>
       <c r="D26" s="6"/>
     </row>
     <row r="27" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>1</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="7"/>
+      <c r="D27" s="9"/>
     </row>
     <row r="28" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>2</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="7"/>
+      <c r="D28" s="9"/>
     </row>
     <row r="29" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <v>3</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="7"/>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="8"/>
+      <c r="C30" s="7"/>
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2">
         <v>1</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="7"/>
+      <c r="D31" s="9"/>
     </row>
     <row r="32" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>2</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="7"/>
+      <c r="D32" s="9"/>
     </row>
     <row r="33" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
         <v>3</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="7"/>
+      <c r="D33" s="9"/>
     </row>
     <row r="34" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="4" t="s">
@@ -2440,19 +2440,19 @@
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="10"/>
+      <c r="C35" s="8"/>
       <c r="D35" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="8"/>
+      <c r="C36" s="7"/>
       <c r="D36" s="6">
         <v>3</v>
       </c>
@@ -2461,34 +2461,34 @@
       <c r="B37" s="2">
         <v>1</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="7"/>
+      <c r="D37" s="9"/>
     </row>
     <row r="38" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <v>2</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="7"/>
+      <c r="D38" s="9"/>
     </row>
     <row r="39" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <v>3</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="7"/>
+      <c r="D39" s="9"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="8"/>
+      <c r="C40" s="7"/>
       <c r="D40" s="6">
         <v>3</v>
       </c>
@@ -2497,68 +2497,70 @@
       <c r="B41" s="2">
         <v>1</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="7"/>
+      <c r="D41" s="9"/>
     </row>
     <row r="42" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <v>2</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D42" s="7"/>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
         <v>3</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D43" s="7"/>
+      <c r="D43" s="9"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="45" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
         <v>1</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D45" s="7"/>
+      <c r="D45" s="9"/>
     </row>
     <row r="46" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
         <v>2</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D46" s="7"/>
+      <c r="D46" s="9"/>
     </row>
     <row r="47" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
         <v>3</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D47" s="7"/>
+      <c r="D47" s="9"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="8"/>
+      <c r="C48" s="7"/>
       <c r="D48" s="6">
         <v>2</v>
       </c>
@@ -2567,62 +2569,62 @@
       <c r="B49" s="2">
         <v>1</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D49" s="7"/>
+      <c r="D49" s="9"/>
     </row>
     <row r="50" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2">
         <v>2</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="7"/>
+      <c r="D50" s="9"/>
     </row>
     <row r="51" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2">
         <v>3</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D51" s="7"/>
+      <c r="D51" s="9"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C52" s="8"/>
+      <c r="C52" s="7"/>
       <c r="D52" s="6"/>
     </row>
     <row r="53" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2">
         <v>1</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D53" s="7"/>
+      <c r="D53" s="9"/>
     </row>
     <row r="54" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="2">
         <v>2</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D54" s="7"/>
+      <c r="D54" s="9"/>
     </row>
     <row r="55" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="2">
         <v>3</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D55" s="7"/>
+      <c r="D55" s="9"/>
     </row>
     <row r="56" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C56" s="4" t="s">
@@ -2630,7 +2632,7 @@
       </c>
       <c r="D56" s="2">
         <f>SUM(D36:D55)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E56" s="2">
         <f>COUNTIF(B37:C55,3)*3</f>
@@ -2638,24 +2640,24 @@
       </c>
       <c r="F56" s="3">
         <f>D56/E56</f>
-        <v>0.53333333333333333</v>
+        <v>0.73333333333333328</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C57" s="10"/>
+      <c r="C57" s="8"/>
       <c r="D57" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C58" s="8"/>
+      <c r="C58" s="7"/>
       <c r="D58" s="6">
         <v>2</v>
       </c>
@@ -2664,102 +2666,102 @@
       <c r="B59" s="2">
         <v>1</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D59" s="7"/>
+      <c r="D59" s="9"/>
     </row>
     <row r="60" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="2">
         <v>2</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D60" s="7"/>
+      <c r="D60" s="9"/>
     </row>
     <row r="61" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2">
         <v>3</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D61" s="7"/>
+      <c r="D61" s="9"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="8" t="s">
+      <c r="B62" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="9"/>
+      <c r="C62" s="10"/>
       <c r="D62" s="6"/>
     </row>
     <row r="63" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2">
         <v>1</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C63" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D63" s="7"/>
+      <c r="D63" s="9"/>
     </row>
     <row r="64" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2">
         <v>2</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C64" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D64" s="7"/>
+      <c r="D64" s="9"/>
     </row>
     <row r="65" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="2">
         <v>3</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C65" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D65" s="7"/>
+      <c r="D65" s="9"/>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B66" s="8" t="s">
+      <c r="B66" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C66" s="8"/>
+      <c r="C66" s="7"/>
       <c r="D66" s="6"/>
     </row>
     <row r="67" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="2">
         <v>1</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="C67" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D67" s="7"/>
+      <c r="D67" s="9"/>
     </row>
     <row r="68" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="2">
         <v>2</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C68" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D68" s="7"/>
+      <c r="D68" s="9"/>
     </row>
     <row r="69" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="2">
         <v>3</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C69" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D69" s="7"/>
+      <c r="D69" s="9"/>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B70" s="8" t="s">
+      <c r="B70" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C70" s="8"/>
+      <c r="C70" s="7"/>
       <c r="D70" s="6">
         <v>3</v>
       </c>
@@ -2768,28 +2770,28 @@
       <c r="B71" s="2">
         <v>1</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="C71" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D71" s="7"/>
+      <c r="D71" s="9"/>
     </row>
     <row r="72" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="2">
         <v>2</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="C72" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D72" s="7"/>
+      <c r="D72" s="9"/>
     </row>
     <row r="73" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="2">
         <v>3</v>
       </c>
-      <c r="C73" s="7" t="s">
+      <c r="C73" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D73" s="7"/>
+      <c r="D73" s="9"/>
     </row>
     <row r="74" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C74" s="4" t="s">
@@ -2814,7 +2816,7 @@
       </c>
       <c r="D75" s="2">
         <f>D74+D56+D34</f>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E75" s="2">
         <f ca="1">SUMIF(C:D,"Total",E:E)</f>
@@ -2822,33 +2824,44 @@
       </c>
       <c r="F75" s="3">
         <f ca="1">D75/E75</f>
-        <v>0.41176470588235292</v>
+        <v>0.47058823529411764</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
@@ -2865,39 +2878,28 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <conditionalFormatting sqref="D35">
     <cfRule type="cellIs" dxfId="158" priority="265" operator="equal">

</xml_diff>